<commit_message>
make changes to database names
</commit_message>
<xml_diff>
--- a/BridgeDatabase.xlsx
+++ b/BridgeDatabase.xlsx
@@ -63,10 +63,10 @@
     <t>ObjectDescription</t>
   </si>
   <si>
-    <t>bridge_inventory</t>
-  </si>
-  <si>
-    <t>bridge_id</t>
+    <t>Bridges</t>
+  </si>
+  <si>
+    <t>BridgeId</t>
   </si>
   <si>
     <t>(newsequentialid())</t>
@@ -75,79 +75,79 @@
     <t>uniqueidentifier</t>
   </si>
   <si>
-    <t>material_design_id</t>
-  </si>
-  <si>
-    <t>material_designs</t>
-  </si>
-  <si>
-    <t>construction_design_id</t>
-  </si>
-  <si>
-    <t>construction_designs</t>
-  </si>
-  <si>
-    <t>functional_class_id</t>
-  </si>
-  <si>
-    <t>functional_classes</t>
-  </si>
-  <si>
-    <t>status_id</t>
-  </si>
-  <si>
-    <t>status_codes</t>
-  </si>
-  <si>
-    <t>county_id</t>
-  </si>
-  <si>
-    <t>counties</t>
-  </si>
-  <si>
-    <t>nbi_num</t>
+    <t>MaterialDesignId</t>
+  </si>
+  <si>
+    <t>MaterialDesigns</t>
+  </si>
+  <si>
+    <t>ConstructionDesignId</t>
+  </si>
+  <si>
+    <t>ConstructionDesigns</t>
+  </si>
+  <si>
+    <t>FunctionalClassId</t>
+  </si>
+  <si>
+    <t>FunctionalClasses</t>
+  </si>
+  <si>
+    <t>StatusId</t>
+  </si>
+  <si>
+    <t>StatusCodes</t>
+  </si>
+  <si>
+    <t>CountyId</t>
+  </si>
+  <si>
+    <t>Counties</t>
+  </si>
+  <si>
+    <t>NbiNumber</t>
   </si>
   <si>
     <t>varchar</t>
   </si>
   <si>
-    <t>rating</t>
+    <t>Rating</t>
   </si>
   <si>
     <t>decimal</t>
   </si>
   <si>
-    <t>route_num</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>intersecting_feature</t>
-  </si>
-  <si>
-    <t>carried_feature</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>built</t>
+    <t>RouteNumber</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>IntersectingFeature</t>
+  </si>
+  <si>
+    <t>CarriedFeature</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Built</t>
   </si>
   <si>
     <t>int</t>
   </si>
   <si>
-    <t>reconstructed</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>construction_design_type</t>
-  </si>
-  <si>
-    <t>county_name</t>
+    <t>Reconstructed</t>
+  </si>
+  <si>
+    <t>TotalLength</t>
+  </si>
+  <si>
+    <t>ConstructionDesignType</t>
+  </si>
+  <si>
+    <t>CountyName</t>
   </si>
   <si>
     <t>Employees</t>
@@ -168,109 +168,109 @@
     <t>Salary</t>
   </si>
   <si>
-    <t>functional_class_type</t>
-  </si>
-  <si>
-    <t>inspection_codes</t>
-  </si>
-  <si>
-    <t>inspection_code_id</t>
-  </si>
-  <si>
-    <t>inspection_code_name</t>
-  </si>
-  <si>
-    <t>inspection_code_desc</t>
-  </si>
-  <si>
-    <t>inspections</t>
-  </si>
-  <si>
-    <t>inspection_id</t>
-  </si>
-  <si>
-    <t>inspector_id</t>
-  </si>
-  <si>
-    <t>inspectors</t>
-  </si>
-  <si>
-    <t>inspection_date</t>
+    <t>FunctionalClassType</t>
+  </si>
+  <si>
+    <t>InspectionCodes</t>
+  </si>
+  <si>
+    <t>InspectionCodeId</t>
+  </si>
+  <si>
+    <t>InspectionCodeName</t>
+  </si>
+  <si>
+    <t>InspectoinCodeDesc</t>
+  </si>
+  <si>
+    <t>Inspections</t>
+  </si>
+  <si>
+    <t>InspectionId</t>
+  </si>
+  <si>
+    <t>InspectorId</t>
+  </si>
+  <si>
+    <t>Inspectors</t>
+  </si>
+  <si>
+    <t>InspectionDate</t>
   </si>
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>deck_inspection_code_id</t>
-  </si>
-  <si>
-    <t>superstructure_inspection_code_id</t>
-  </si>
-  <si>
-    <t>substructure_inspection_code_id</t>
-  </si>
-  <si>
-    <t>inspection_notes</t>
-  </si>
-  <si>
-    <t>inspector_first</t>
-  </si>
-  <si>
-    <t>inspector_last</t>
-  </si>
-  <si>
-    <t>inspector_org</t>
-  </si>
-  <si>
-    <t>inspector_cert_effective</t>
-  </si>
-  <si>
-    <t>inspector_cert_expires</t>
-  </si>
-  <si>
-    <t>maintenace</t>
-  </si>
-  <si>
-    <t>maint_id</t>
-  </si>
-  <si>
-    <t>maint_action_id</t>
-  </si>
-  <si>
-    <t>maintenance_actions</t>
-  </si>
-  <si>
-    <t>maint_projected_start</t>
-  </si>
-  <si>
-    <t>maint_projected_end</t>
-  </si>
-  <si>
-    <t>maint_actual_start</t>
-  </si>
-  <si>
-    <t>maint_actual_end</t>
-  </si>
-  <si>
-    <t>maint_proj_cost</t>
-  </si>
-  <si>
-    <t>maint_actual_cost</t>
-  </si>
-  <si>
-    <t>maint_notes</t>
-  </si>
-  <si>
-    <t>maint_inspector_notes</t>
-  </si>
-  <si>
-    <t>maint_action_name</t>
-  </si>
-  <si>
-    <t>material_design_type</t>
-  </si>
-  <si>
-    <t>status_name</t>
+    <t>DeckInspectoinCodeId</t>
+  </si>
+  <si>
+    <t>SuperstructureInspectionCodeId</t>
+  </si>
+  <si>
+    <t>SubstructureInspectionCodeId</t>
+  </si>
+  <si>
+    <t>InspectionNotes</t>
+  </si>
+  <si>
+    <t>InspectorFirst</t>
+  </si>
+  <si>
+    <t>InspectorLast</t>
+  </si>
+  <si>
+    <t>InspectorOrg</t>
+  </si>
+  <si>
+    <t>InspectorCertEffective</t>
+  </si>
+  <si>
+    <t>InspectorCertExpires</t>
+  </si>
+  <si>
+    <t>MaintenanceActions</t>
+  </si>
+  <si>
+    <t>MaintenanceActionId</t>
+  </si>
+  <si>
+    <t>MaintenanceActionName</t>
+  </si>
+  <si>
+    <t>MaintenanceRecords</t>
+  </si>
+  <si>
+    <t>MaintenaceId</t>
+  </si>
+  <si>
+    <t>MaintenanceProjectedStart</t>
+  </si>
+  <si>
+    <t>MaintenanceProjectedEnd</t>
+  </si>
+  <si>
+    <t>MaintenanceActualStart</t>
+  </si>
+  <si>
+    <t>MaintenanceActualEnd</t>
+  </si>
+  <si>
+    <t>MantenanceProjectedCost</t>
+  </si>
+  <si>
+    <t>MaintenanceActualCost</t>
+  </si>
+  <si>
+    <t>MaintenanceNotes</t>
+  </si>
+  <si>
+    <t>InspectorNotes</t>
+  </si>
+  <si>
+    <t>MaterialDesignType</t>
+  </si>
+  <si>
+    <t>StatusName</t>
   </si>
   <si>
     <t>sysdiagrams</t>
@@ -611,15 +611,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:N79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
@@ -679,7 +679,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -778,7 +778,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
@@ -1343,7 +1343,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>27</v>
@@ -1369,7 +1369,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>27</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
         <v>43</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
         <v>43</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
         <v>43</v>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
         <v>43</v>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
         <v>43</v>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
         <v>23</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
         <v>23</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
         <v>50</v>
@@ -1709,7 +1709,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
         <v>50</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
         <v>50</v>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
         <v>50</v>
@@ -1808,7 +1808,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
         <v>54</v>
@@ -1834,7 +1834,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
         <v>54</v>
@@ -1869,7 +1869,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
         <v>54</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
         <v>54</v>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B41" t="s">
         <v>54</v>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
         <v>54</v>
@@ -2015,7 +2015,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
         <v>54</v>
@@ -2053,7 +2053,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B44" t="s">
         <v>54</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B45" t="s">
         <v>54</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B46" t="s">
         <v>57</v>
@@ -2149,7 +2149,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B47" t="s">
         <v>57</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="B48" t="s">
         <v>57</v>
@@ -2216,7 +2216,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B49" t="s">
         <v>57</v>
@@ -2248,7 +2248,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B50" t="s">
         <v>57</v>
@@ -2280,7 +2280,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B51" t="s">
         <v>57</v>
@@ -2312,7 +2312,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B52" t="s">
         <v>57</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="B53" t="s">
         <v>69</v>
@@ -2370,7 +2370,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B54" t="s">
         <v>69</v>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B55" t="s">
         <v>69</v>
@@ -2420,10 +2420,10 @@
         <v>0</v>
       </c>
       <c r="G55" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -2432,34 +2432,22 @@
         <v>0</v>
       </c>
       <c r="K55">
-        <v>1</v>
-      </c>
-      <c r="L55" t="s">
-        <v>72</v>
-      </c>
-      <c r="M55" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="D56">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F56">
         <v>0</v>
       </c>
-      <c r="G56" t="s">
-        <v>17</v>
-      </c>
       <c r="H56">
         <v>0</v>
       </c>
@@ -2470,33 +2458,30 @@
         <v>0</v>
       </c>
       <c r="K56">
-        <v>1</v>
-      </c>
-      <c r="L56" t="s">
-        <v>57</v>
-      </c>
-      <c r="M56" t="s">
-        <v>56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C57" t="s">
         <v>73</v>
       </c>
       <c r="D57">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>16</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
       <c r="G57" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -2505,7 +2490,7 @@
         <v>0</v>
       </c>
       <c r="J57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -2513,54 +2498,60 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B58" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58" t="s">
+        <v>17</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58" t="s">
         <v>69</v>
       </c>
-      <c r="C58" t="s">
-        <v>74</v>
-      </c>
-      <c r="D58">
-        <v>5</v>
-      </c>
-      <c r="F58">
-        <v>0</v>
-      </c>
-      <c r="G58" t="s">
-        <v>59</v>
-      </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
-      <c r="I58">
-        <v>0</v>
-      </c>
-      <c r="J58">
-        <v>0</v>
-      </c>
-      <c r="K58">
-        <v>0</v>
+      <c r="M58" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C59" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="D59">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -2572,24 +2563,30 @@
         <v>0</v>
       </c>
       <c r="K59">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L59" t="s">
+        <v>57</v>
+      </c>
+      <c r="M59" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D60">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60" t="s">
         <v>59</v>
@@ -2609,22 +2606,22 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C61" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D61">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F61">
         <v>0</v>
       </c>
       <c r="G61" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -2641,22 +2638,22 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D62">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F62">
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -2673,25 +2670,25 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C63" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D63">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F63">
         <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="H63">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I63">
         <v>0</v>
@@ -2705,25 +2702,25 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C64" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D64">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H64">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I64">
         <v>0</v>
@@ -2737,16 +2734,22 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="B65" t="s">
         <v>72</v>
       </c>
+      <c r="C65" t="s">
+        <v>79</v>
+      </c>
       <c r="D65">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G65" t="s">
+        <v>31</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -2763,34 +2766,31 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
         <v>72</v>
       </c>
       <c r="C66" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="E66" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="I66">
         <v>0</v>
       </c>
       <c r="J66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K66">
         <v>0</v>
@@ -2798,7 +2798,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
         <v>72</v>
@@ -2807,16 +2807,16 @@
         <v>81</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67" t="s">
         <v>29</v>
       </c>
       <c r="H67">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="I67">
         <v>0</v>
@@ -2830,7 +2830,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>19</v>
@@ -2856,7 +2856,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>19</v>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>19</v>
@@ -2923,7 +2923,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>25</v>
@@ -2949,7 +2949,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>25</v>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>25</v>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>84</v>
@@ -3042,7 +3042,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>84</v>
@@ -3074,7 +3074,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>84</v>
@@ -3106,7 +3106,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>84</v>
@@ -3138,7 +3138,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>84</v>
@@ -3170,7 +3170,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
finish work with entity framework
</commit_message>
<xml_diff>
--- a/BridgeDatabase.xlsx
+++ b/BridgeDatabase.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="91">
   <si>
     <t>RowID</t>
   </si>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
         <v>43</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
         <v>43</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
         <v>43</v>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
         <v>43</v>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
         <v>43</v>
@@ -2214,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>43</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>44</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>45</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>46</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>47</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>48</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>49</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>50</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>51</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>52</v>
       </c>
@@ -2525,16 +2525,10 @@
         <v>0</v>
       </c>
       <c r="K58">
-        <v>1</v>
-      </c>
-      <c r="L58" t="s">
-        <v>69</v>
-      </c>
-      <c r="M58" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>53</v>
       </c>
@@ -2563,16 +2557,10 @@
         <v>0</v>
       </c>
       <c r="K59">
-        <v>1</v>
-      </c>
-      <c r="L59" t="s">
-        <v>57</v>
-      </c>
-      <c r="M59" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>54</v>
       </c>
@@ -2604,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>55</v>
       </c>
@@ -2636,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>56</v>
       </c>
@@ -2668,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>57</v>
       </c>
@@ -2700,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>58</v>
       </c>
@@ -2830,7 +2818,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B68" t="s">
         <v>19</v>
@@ -2856,7 +2844,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B69" t="s">
         <v>19</v>
@@ -2891,7 +2879,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B70" t="s">
         <v>19</v>
@@ -2923,7 +2911,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B71" t="s">
         <v>25</v>
@@ -2949,7 +2937,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B72" t="s">
         <v>25</v>
@@ -2984,7 +2972,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B73" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
change some more names
</commit_message>
<xml_diff>
--- a/BridgeDatabase.xlsx
+++ b/BridgeDatabase.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="92">
   <si>
     <t>RowID</t>
   </si>
@@ -99,6 +99,9 @@
     <t>StatusCodes</t>
   </si>
   <si>
+    <t>StatusCodeId</t>
+  </si>
+  <si>
     <t>CountyId</t>
   </si>
   <si>
@@ -180,7 +183,7 @@
     <t>InspectionCodeName</t>
   </si>
   <si>
-    <t>InspectoinCodeDesc</t>
+    <t>InspectionCodeDesc</t>
   </si>
   <si>
     <t>Inspections</t>
@@ -201,7 +204,7 @@
     <t>date</t>
   </si>
   <si>
-    <t>DeckInspectoinCodeId</t>
+    <t>DeckInspectionCodeId</t>
   </si>
   <si>
     <t>SuperstructureInspectionCodeId</t>
@@ -240,7 +243,7 @@
     <t>MaintenanceRecords</t>
   </si>
   <si>
-    <t>MaintenaceId</t>
+    <t>MaintenanceRecordId</t>
   </si>
   <si>
     <t>MaintenanceProjectedStart</t>
@@ -255,7 +258,7 @@
     <t>MaintenanceActualEnd</t>
   </si>
   <si>
-    <t>MantenanceProjectedCost</t>
+    <t>MaintenanceProjectedCost</t>
   </si>
   <si>
     <t>MaintenanceActualCost</t>
@@ -887,7 +890,7 @@
         <v>25</v>
       </c>
       <c r="M7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -898,7 +901,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -922,10 +925,10 @@
         <v>1</v>
       </c>
       <c r="L8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" t="s">
         <v>27</v>
-      </c>
-      <c r="M8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -936,7 +939,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -945,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H9">
         <v>100</v>
@@ -968,7 +971,7 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -977,7 +980,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1000,7 +1003,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -1009,7 +1012,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H11">
         <v>25</v>
@@ -1032,7 +1035,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1041,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H12">
         <v>50</v>
@@ -1064,7 +1067,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13">
         <v>11</v>
@@ -1073,7 +1076,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H13">
         <v>255</v>
@@ -1096,7 +1099,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14">
         <v>12</v>
@@ -1105,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H14">
         <v>255</v>
@@ -1128,7 +1131,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15">
         <v>13</v>
@@ -1137,7 +1140,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H15">
         <v>255</v>
@@ -1160,7 +1163,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>14</v>
@@ -1169,7 +1172,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1192,7 +1195,7 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>15</v>
@@ -1201,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1224,7 +1227,7 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18">
         <v>16</v>
@@ -1233,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1317,7 +1320,7 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -1326,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H21">
         <v>50</v>
@@ -1346,7 +1349,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1372,10 +1375,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
         <v>27</v>
-      </c>
-      <c r="C23" t="s">
-        <v>26</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1407,10 +1410,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -1419,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H24">
         <v>50</v>
@@ -1439,7 +1442,7 @@
         <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1465,10 +1468,10 @@
         <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1477,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1497,10 +1500,10 @@
         <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D27">
         <v>2</v>
@@ -1509,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H27">
         <v>50</v>
@@ -1529,10 +1532,10 @@
         <v>71</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -1541,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H28">
         <v>50</v>
@@ -1561,10 +1564,10 @@
         <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D29">
         <v>4</v>
@@ -1573,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -1657,7 +1660,7 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -1666,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H32">
         <v>50</v>
@@ -1686,7 +1689,7 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1712,10 +1715,10 @@
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1747,10 +1750,10 @@
         <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -1759,7 +1762,7 @@
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H35">
         <v>50</v>
@@ -1779,10 +1782,10 @@
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -1791,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H36">
         <v>400</v>
@@ -1811,7 +1814,7 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1837,10 +1840,10 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1872,7 +1875,7 @@
         <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
         <v>15</v>
@@ -1910,10 +1913,10 @@
         <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D40">
         <v>3</v>
@@ -1937,10 +1940,10 @@
         <v>1</v>
       </c>
       <c r="L40" t="s">
+        <v>58</v>
+      </c>
+      <c r="M40" t="s">
         <v>57</v>
-      </c>
-      <c r="M40" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -1948,10 +1951,10 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D41">
         <v>4</v>
@@ -1960,7 +1963,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -1980,10 +1983,10 @@
         <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D42">
         <v>5</v>
@@ -2007,10 +2010,10 @@
         <v>1</v>
       </c>
       <c r="L42" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -2018,10 +2021,10 @@
         <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D43">
         <v>6</v>
@@ -2045,10 +2048,10 @@
         <v>1</v>
       </c>
       <c r="L43" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M43" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2056,10 +2059,10 @@
         <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D44">
         <v>7</v>
@@ -2083,10 +2086,10 @@
         <v>1</v>
       </c>
       <c r="L44" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M44" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -2094,10 +2097,10 @@
         <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C45" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D45">
         <v>8</v>
@@ -2106,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H45">
         <v>2000</v>
@@ -2126,7 +2129,7 @@
         <v>40</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2152,10 +2155,10 @@
         <v>41</v>
       </c>
       <c r="B47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" t="s">
         <v>57</v>
-      </c>
-      <c r="C47" t="s">
-        <v>56</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -2187,10 +2190,10 @@
         <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D48">
         <v>2</v>
@@ -2199,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H48">
         <v>50</v>
@@ -2219,10 +2222,10 @@
         <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D49">
         <v>3</v>
@@ -2231,7 +2234,7 @@
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H49">
         <v>50</v>
@@ -2251,10 +2254,10 @@
         <v>44</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D50">
         <v>4</v>
@@ -2263,7 +2266,7 @@
         <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H50">
         <v>50</v>
@@ -2283,10 +2286,10 @@
         <v>45</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D51">
         <v>5</v>
@@ -2295,7 +2298,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -2315,10 +2318,10 @@
         <v>46</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D52">
         <v>6</v>
@@ -2327,7 +2330,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -2347,7 +2350,7 @@
         <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2373,10 +2376,10 @@
         <v>48</v>
       </c>
       <c r="B54" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C54" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -2408,10 +2411,10 @@
         <v>49</v>
       </c>
       <c r="B55" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C55" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D55">
         <v>2</v>
@@ -2420,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H55">
         <v>50</v>
@@ -2440,7 +2443,7 @@
         <v>50</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2466,10 +2469,10 @@
         <v>51</v>
       </c>
       <c r="B57" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C57" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -2501,10 +2504,10 @@
         <v>52</v>
       </c>
       <c r="B58" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D58">
         <v>2</v>
@@ -2533,10 +2536,10 @@
         <v>53</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C59" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D59">
         <v>3</v>
@@ -2565,10 +2568,10 @@
         <v>54</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C60" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D60">
         <v>4</v>
@@ -2577,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -2597,10 +2600,10 @@
         <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C61" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D61">
         <v>5</v>
@@ -2609,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -2629,10 +2632,10 @@
         <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C62" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D62">
         <v>6</v>
@@ -2641,7 +2644,7 @@
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -2661,10 +2664,10 @@
         <v>57</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C63" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D63">
         <v>7</v>
@@ -2673,7 +2676,7 @@
         <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -2693,10 +2696,10 @@
         <v>58</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C64" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D64">
         <v>8</v>
@@ -2705,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -2725,10 +2728,10 @@
         <v>59</v>
       </c>
       <c r="B65" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C65" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D65">
         <v>9</v>
@@ -2737,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="G65" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -2757,10 +2760,10 @@
         <v>60</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C66" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D66">
         <v>10</v>
@@ -2769,7 +2772,7 @@
         <v>1</v>
       </c>
       <c r="G66" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H66">
         <v>1000</v>
@@ -2789,10 +2792,10 @@
         <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C67" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D67">
         <v>11</v>
@@ -2801,7 +2804,7 @@
         <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H67">
         <v>1000</v>
@@ -2885,7 +2888,7 @@
         <v>19</v>
       </c>
       <c r="C70" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D70">
         <v>2</v>
@@ -2894,7 +2897,7 @@
         <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H70">
         <v>50</v>
@@ -2943,7 +2946,7 @@
         <v>25</v>
       </c>
       <c r="C72" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -2978,7 +2981,7 @@
         <v>25</v>
       </c>
       <c r="C73" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D73">
         <v>2</v>
@@ -2987,7 +2990,7 @@
         <v>0</v>
       </c>
       <c r="G73" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H73">
         <v>50</v>
@@ -3007,7 +3010,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -3033,10 +3036,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -3045,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="G75" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H75">
         <v>128</v>
@@ -3065,10 +3068,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C76" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D76">
         <v>2</v>
@@ -3077,7 +3080,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -3097,10 +3100,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D77">
         <v>3</v>
@@ -3109,7 +3112,7 @@
         <v>0</v>
       </c>
       <c r="G77" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -3129,10 +3132,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C78" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D78">
         <v>4</v>
@@ -3141,7 +3144,7 @@
         <v>1</v>
       </c>
       <c r="G78" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -3161,10 +3164,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C79" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D79">
         <v>5</v>
@@ -3173,7 +3176,7 @@
         <v>1</v>
       </c>
       <c r="G79" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H79">
         <v>-1</v>

</xml_diff>